<commit_message>
Refactor optimization model and result extraction
- Updated the optimization model to improve the handling of offers and demand.
- Enhanced the result extraction function to include detailed statistics and summaries.
- Added functionality to calculate total assigned energy and deficits more accurately.
- Improved error handling and logging throughout the process.
- Updated the export functionality to include both indexed and non-indexed price summaries.
- Modified the way statistics are calculated and stored in Excel files.
- Adjusted the way offers are prioritized and filtered for better clarity and performance.
</commit_message>
<xml_diff>
--- a/output/estadisticas_ofertas.xlsx
+++ b/output/estadisticas_ofertas.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,84 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IDENTIFICADOR</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL ASIGNADO (kWh)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PRECIO PROMEDIO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>COSTO TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>OFERTA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OP1_Wide -AES</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>415000000.0000029</v>
+      </c>
+      <c r="D2" t="n">
+        <v>135.2911123114241</v>
+      </c>
+      <c r="E2" t="n">
+        <v>56145811609.24137</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TODAS LAS OFERTAS</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>415000000.0000029</v>
+      </c>
+      <c r="D3" t="n">
+        <v>135.2911123114241</v>
+      </c>
+      <c r="E3" t="n">
+        <v>56145811609.24137</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de como mostrar los resultados finasles
</commit_message>
<xml_diff>
--- a/output/estadisticas_ofertas.xlsx
+++ b/output/estadisticas_ofertas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,34 +472,76 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>415000000.0000029</v>
+        <v>190000000.0000004</v>
       </c>
       <c r="D2" t="n">
-        <v>135.2911123114241</v>
+        <v>105.1172485027671</v>
       </c>
       <c r="E2" t="n">
-        <v>56145811609.24137</v>
+        <v>19972277215.52578</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>OFERTA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OP1_Wide -ISAGEN</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>190000000.0000004</v>
+      </c>
+      <c r="D3" t="n">
+        <v>54.47866916837214</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10350947141.99072</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>OFERTA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OP1_Wide- EPM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>916608868</v>
+      </c>
+      <c r="D4" t="n">
+        <v>57.83386399818058</v>
+      </c>
+      <c r="E4" t="n">
+        <v>53011032611.43826</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>TODAS LAS OFERTAS</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>415000000.0000029</v>
-      </c>
-      <c r="D3" t="n">
-        <v>135.2911123114241</v>
-      </c>
-      <c r="E3" t="n">
-        <v>56145811609.24137</v>
+      <c r="C5" t="n">
+        <v>1296608868.000001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>64.27092936476407</v>
+      </c>
+      <c r="E5" t="n">
+        <v>83334256968.95476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejora la función de exportación de resultados para incluir información de ofertas rechazadas por precio y optimizar la lectura de datos originales. Se actualizan las proyecciones de indexadores y se realizan ajustes en la gestión de precios SICEP. Se eliminan hojas innecesarias y se corrigen errores de lectura de datos.
</commit_message>
<xml_diff>
--- a/output/estadisticas_ofertas.xlsx
+++ b/output/estadisticas_ofertas.xlsx
@@ -472,13 +472,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>190000000.0000004</v>
+        <v>415000000.0000029</v>
       </c>
       <c r="D2" t="n">
-        <v>105.1172485027671</v>
+        <v>129.5714928739288</v>
       </c>
       <c r="E2" t="n">
-        <v>19972277215.52578</v>
+        <v>53772169542.68082</v>
       </c>
     </row>
     <row r="3">
@@ -493,13 +493,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>190000000.0000004</v>
+        <v>459458287.0000031</v>
       </c>
       <c r="D3" t="n">
-        <v>54.47866916837214</v>
+        <v>81.67845026912242</v>
       </c>
       <c r="E3" t="n">
-        <v>10350947141.99072</v>
+        <v>37527840845.46593</v>
       </c>
     </row>
     <row r="4">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>916608868</v>
+        <v>880608868</v>
       </c>
       <c r="D4" t="n">
-        <v>57.83386399818058</v>
+        <v>53.76483966340702</v>
       </c>
       <c r="E4" t="n">
-        <v>53011032611.43826</v>
+        <v>47345794594.19435</v>
       </c>
     </row>
     <row r="5">
@@ -535,13 +535,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1296608868.000001</v>
+        <v>1755067155.000006</v>
       </c>
       <c r="D5" t="n">
-        <v>64.27092936476407</v>
+        <v>78.9974358458897</v>
       </c>
       <c r="E5" t="n">
-        <v>83334256968.95476</v>
+        <v>138645804982.3411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>